<commit_message>
mudanças planilha de conformidade
</commit_message>
<xml_diff>
--- a/figuras/conformance.xlsx
+++ b/figuras/conformance.xlsx
@@ -441,11 +441,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2014853440"/>
-        <c:axId val="-1846656752"/>
+        <c:axId val="1673234752"/>
+        <c:axId val="1673236384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2014853440"/>
+        <c:axId val="1673234752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -488,7 +488,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1846656752"/>
+        <c:crossAx val="1673236384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -496,7 +496,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1846656752"/>
+        <c:axId val="1673236384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -547,7 +547,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2014853440"/>
+        <c:crossAx val="1673234752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1472,7 +1472,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Reescrito a seção sobre teste de conformidade e resumo foi ampliado (Necéssario revisão)
</commit_message>
<xml_diff>
--- a/figuras/conformance.xlsx
+++ b/figuras/conformance.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -400,7 +400,7 @@
                   <c:v>0.94667000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.91488999999999998</c:v>
+                  <c:v>0.97872000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.91918999999999995</c:v>
@@ -412,19 +412,19 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.84677000000000002</c:v>
+                  <c:v>0.9758</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.89654999999999996</c:v>
+                  <c:v>0.98850000000000005</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.90788999999999997</c:v>
+                  <c:v>0.97377999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -441,11 +441,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1673234752"/>
-        <c:axId val="1673236384"/>
+        <c:axId val="-1797382400"/>
+        <c:axId val="-1797387840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1673234752"/>
+        <c:axId val="-1797382400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -488,7 +488,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1673236384"/>
+        <c:crossAx val="-1797387840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -496,7 +496,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1673236384"/>
+        <c:axId val="-1797387840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -547,7 +547,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1673234752"/>
+        <c:crossAx val="-1797382400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1471,8 +1471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1510,7 +1510,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="5">
-        <v>0.91488999999999998</v>
+        <v>0.97872000000000003</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -1554,7 +1554,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="5">
-        <v>0.84677000000000002</v>
+        <v>0.9758</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -1576,7 +1576,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="5">
-        <v>0.89654999999999996</v>
+        <v>0.98850000000000005</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -1598,7 +1598,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="5">
-        <v>0.90788999999999997</v>
+        <v>0.97377999999999998</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1607,7 +1607,7 @@
       </c>
       <c r="C13" s="7">
         <f>AVERAGE(C2,C3,C4,C5,C6,C7,C8,C9,C10,C11)</f>
-        <v>0.94319600000000003</v>
+        <v>0.97826599999999997</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>